<commit_message>
been trying to work on how to display tables in subplot
</commit_message>
<xml_diff>
--- a/riket2023_åk9_np.xlsx
+++ b/riket2023_åk9_np.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Engelska"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="40">
   <si>
     <t>Grundskolan - Resultat nationella prov årskurs 9, provbetyg per kön - Engelska, Matematik och Svenska/svenska som andraspråk</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Svenska</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
   <si>
     <t>Matematik</t>
@@ -144,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +160,12 @@
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -175,7 +184,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -218,28 +227,28 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -632,7 +641,7 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A10" ySplit="9" xSplit="0"/>
     </sheetView>
   </sheetViews>
@@ -694,7 +703,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
@@ -802,7 +811,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -837,7 +846,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -872,7 +881,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -907,7 +916,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -962,7 +971,7 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A10" ySplit="9" xSplit="0"/>
     </sheetView>
   </sheetViews>
@@ -982,7 +991,9 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="B1" s="1"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1024,7 +1035,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
@@ -1254,13 +1265,13 @@
         <v>25</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I13" s="11">
         <v>14.1</v>

</xml_diff>

<commit_message>
Switched from table to bar chart in subplots
Initially created a table with all results, but realized it should be a bar chart.
Now implemented subplots with bar charts instead.
</commit_message>
<xml_diff>
--- a/riket2023_åk9_np.xlsx
+++ b/riket2023_åk9_np.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Engelska"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="39">
   <si>
     <t>Grundskolan - Resultat nationella prov årskurs 9, provbetyg per kön - Engelska, Matematik och Svenska/svenska som andraspråk</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>Skolverket</t>
-  </si>
-  <si>
-    <t>..</t>
   </si>
   <si>
     <t>Svenska</t>
@@ -147,7 +144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,7 +161,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -180,12 +177,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -216,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -244,12 +235,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -649,15 +634,15 @@
   <cols>
     <col min="1" max="1" style="3" width="10.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="28.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="12.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -703,7 +688,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
@@ -818,31 +803,31 @@
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="4">
         <v>106941</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="4">
         <v>51864</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="4">
         <v>55077</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="5">
         <v>97</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="5">
         <v>97.1</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="5">
         <v>97</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="5">
         <v>15.7</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="5">
         <v>15.8</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="5">
         <v>15.7</v>
       </c>
     </row>
@@ -853,31 +838,31 @@
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="4">
         <v>84310</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="4">
         <v>40675</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="4">
         <v>43635</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="5">
         <v>96.6</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="5">
         <v>96.6</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="5">
         <v>96.6</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="5">
         <v>15.4</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="5">
         <v>15.5</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="5">
         <v>15.4</v>
       </c>
     </row>
@@ -888,31 +873,31 @@
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="4">
         <v>22582</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="4">
         <v>11165</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="4">
         <v>11417</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="5">
         <v>98.7</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="5">
         <v>98.8</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="5">
         <v>98.7</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="5">
         <v>16.9</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="5">
         <v>17</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="5">
         <v>16.8</v>
       </c>
     </row>
@@ -923,31 +908,31 @@
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="4">
         <v>49</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="4">
         <v>24</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="4">
         <v>25</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="5">
         <v>100</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="5">
         <v>100</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="5">
         <v>100</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="5">
         <v>18.5</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="5">
         <v>18.9</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="5">
         <v>18.2</v>
       </c>
     </row>
@@ -971,7 +956,7 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A10" ySplit="9" xSplit="0"/>
     </sheetView>
   </sheetViews>
@@ -979,20 +964,20 @@
   <cols>
     <col min="1" max="1" style="3" width="10.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="12.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="4"/>
@@ -1035,7 +1020,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
@@ -1150,31 +1135,31 @@
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="4">
         <v>106766</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="4">
         <v>51548</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="4">
         <v>55218</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="5">
         <v>89.1</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="5">
         <v>88.7</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="5">
         <v>89.5</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="5">
         <v>11.9</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="5">
         <v>11.8</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="5">
         <v>12</v>
       </c>
     </row>
@@ -1185,31 +1170,31 @@
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="4">
         <v>84163</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="4">
         <v>40386</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="4">
         <v>43777</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="5">
         <v>88.1</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="5">
         <v>87.7</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="5">
         <v>88.5</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="5">
         <v>11.6</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="5">
         <v>11.5</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="5">
         <v>11.7</v>
       </c>
     </row>
@@ -1220,31 +1205,31 @@
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="4">
         <v>22553</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="4">
         <v>11137</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="4">
         <v>11416</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="5">
         <v>92.9</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="5">
         <v>92.2</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="5">
         <v>93.5</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="5">
         <v>13</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="5">
         <v>12.8</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="5">
         <v>13.1</v>
       </c>
     </row>
@@ -1255,31 +1240,31 @@
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="4">
         <v>50</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="4">
         <v>25</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="4">
         <v>25</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="11">
+      <c r="F13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="5">
         <v>14.1</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="5">
         <v>13.5</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="5">
         <v>14.7</v>
       </c>
     </row>
@@ -1311,15 +1296,15 @@
   <cols>
     <col min="1" max="1" style="3" width="36.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="12.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1365,7 +1350,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
@@ -1480,31 +1465,31 @@
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="4">
         <v>93225</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="4">
         <v>45800</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="4">
         <v>47425</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="5">
         <v>96.1</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="5">
         <v>97.9</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="5">
         <v>94.4</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="5">
         <v>13.6</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="5">
         <v>14.5</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="5">
         <v>12.7</v>
       </c>
     </row>
@@ -1515,31 +1500,31 @@
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="4">
         <v>72771</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="4">
         <v>35484</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="4">
         <v>37287</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="5">
         <v>95.7</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="5">
         <v>97.6</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="5">
         <v>93.8</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="5">
         <v>13.3</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="5">
         <v>14.3</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="5">
         <v>12.4</v>
       </c>
     </row>
@@ -1550,31 +1535,31 @@
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="4">
         <v>20414</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="4">
         <v>10297</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="4">
         <v>10117</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="5">
         <v>97.6</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="5">
         <v>98.7</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="5">
         <v>96.6</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="5">
         <v>14.4</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="5">
         <v>15.2</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="5">
         <v>13.5</v>
       </c>
     </row>
@@ -1585,31 +1570,31 @@
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="4">
         <v>40</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="4">
         <v>19</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="4">
         <v>21</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="5">
         <v>100</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="5">
         <v>100</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="5">
         <v>100</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="5">
         <v>15</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="5">
         <v>15.9</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="5">
         <v>14.2</v>
       </c>
     </row>
@@ -1633,7 +1618,7 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A10" ySplit="9" xSplit="0"/>
     </sheetView>
   </sheetViews>
@@ -1641,15 +1626,15 @@
   <cols>
     <col min="1" max="1" style="3" width="10.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="12.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1810,31 +1795,31 @@
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="4">
         <v>14092</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="4">
         <v>6447</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="4">
         <v>7645</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="5">
         <v>77.7</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="5">
         <v>81.6</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="5">
         <v>74.3</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="5">
         <v>9.4</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="5">
         <v>10.2</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="5">
         <v>8.7</v>
       </c>
     </row>
@@ -1845,31 +1830,31 @@
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="4">
         <v>11963</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="4">
         <v>5495</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="4">
         <v>6468</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="5">
         <v>75.9</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="5">
         <v>80</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="5">
         <v>72.4</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="5">
         <v>9</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="5">
         <v>9.9</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="5">
         <v>8.3</v>
       </c>
     </row>
@@ -1880,31 +1865,31 @@
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="4">
         <v>2122</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="4">
         <v>949</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="4">
         <v>1173</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="5">
         <v>87.7</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="5">
         <v>90.9</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="5">
         <v>85.2</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="5">
         <v>11.1</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="5">
         <v>12</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="5">
         <v>10.4</v>
       </c>
     </row>
@@ -1915,32 +1900,32 @@
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>34</v>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>